<commit_message>
Completing phases to end Client Order
</commit_message>
<xml_diff>
--- a/pandas_excercises/perform_analysis1/personas_sucursales/outputs/personas_limpias.xlsx
+++ b/pandas_excercises/perform_analysis1/personas_sucursales/outputs/personas_limpias.xlsx
@@ -463,11 +463,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -477,20 +477,16 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Adulto</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>José</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -502,45 +498,45 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Jóven</t>
+          <t>Mayor</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sofía</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rosario</t>
+          <t>Salta</t>
         </is>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Adolescente</t>
+          <t>Adulto</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tomás</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mendoza</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -548,22 +544,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jóven</t>
+          <t>Adulto</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Valentina</t>
+          <t>Agustina</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -578,38 +574,38 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Federico</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Adolescente</t>
+          <t>Jóven</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Agustina</t>
+          <t>Martina</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Mendoza</t>
         </is>
       </c>
       <c r="D8" t="b">
@@ -624,15 +620,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nicolás</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rosario</t>
+          <t>Mendoza</t>
         </is>
       </c>
       <c r="D9" t="b">
@@ -647,11 +643,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Martina</t>
+          <t>Tomás</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -670,15 +666,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lucía</t>
+          <t>Nicolás</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Rosario</t>
         </is>
       </c>
       <c r="D11" t="b">
@@ -693,15 +689,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Valentina</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="D12" t="b">
@@ -709,22 +705,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Adulto</t>
+          <t>Jóven</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>José</t>
+          <t>Lucía</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="D13" t="b">
@@ -732,51 +728,55 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Mayor</t>
+          <t>Jóven</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Federico</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mendoza</t>
+          <t>Salta</t>
         </is>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Jóven</t>
+          <t>Adolescente</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Error</t>
+          <t>Sofía</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Rosario</t>
         </is>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Adolescente</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>